<commit_message>
People can move now. Will register live on other's screens
</commit_message>
<xml_diff>
--- a/testmap2.xlsx
+++ b/testmap2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nepplnj\Documents\GitHub\testing-dnd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93858527-9497-4BEF-9AE3-6F8E85CE0633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06640466-0841-4C00-AF6F-7D350DB339E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{783A9779-C77F-4BF2-BC3A-D02569825052}"/>
+    <workbookView xWindow="1440" yWindow="1440" windowWidth="19200" windowHeight="11260" xr2:uid="{783A9779-C77F-4BF2-BC3A-D02569825052}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,7 +405,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -468,10 +468,10 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -518,10 +518,10 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <v>1</v>

</xml_diff>